<commit_message>
them log out, import excel cau hoi
</commit_message>
<xml_diff>
--- a/ImportExcel/CauHoi.xlsx
+++ b/ImportExcel/CauHoi.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\UTT_C_SHARP_AppThiTracNghiem\ImportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87969D7D-0260-4969-B0EC-D1DAE345EFA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB183737-550D-4DD4-BA16-116E72EB4194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{598F657F-1048-4F4C-B105-0694A7CEF035}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -35,48 +34,387 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>Đáp án đúng</t>
-  </si>
-  <si>
-    <t>Đáp án D</t>
-  </si>
-  <si>
-    <t>Đáp án C</t>
-  </si>
-  <si>
-    <t>Đáp án B</t>
-  </si>
-  <si>
-    <t>Đáp án A</t>
-  </si>
-  <si>
-    <t>Nội dung câu hỏi</t>
-  </si>
-  <si>
-    <t>Thủ đô của Việt Nam là?</t>
-  </si>
-  <si>
-    <t>Hồ Chí Minh</t>
-  </si>
-  <si>
-    <t>Đà Nẵng</t>
-  </si>
-  <si>
-    <t>Hải Phòng</t>
-  </si>
-  <si>
-    <t>2 + 2 bằng mấy ?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="127">
   <si>
     <t>C</t>
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>NoiDungCauHoi</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ lập trình C# được phát triển bởi công ty nào?</t>
+  </si>
+  <si>
+    <t>Trong C#, từ khóa nào được sử dụng để khai báo một biến không thể thay đổi giá trị?</t>
+  </si>
+  <si>
+    <t>Phương thức Main() trong C# có vai trò gì?</t>
+  </si>
+  <si>
+    <t>Kiểu dữ liệu nào trong C# được sử dụng để lưu trữ giá trị true/false?</t>
+  </si>
+  <si>
+    <t>Namespace trong C# có tác dụng gì?</t>
+  </si>
+  <si>
+    <t>Từ khóa "using" trong C# được sử dụng để làm gì?</t>
+  </si>
+  <si>
+    <t>Trong C#, để kế thừa từ một lớp khác ta sử dụng ký tự gì?</t>
+  </si>
+  <si>
+    <t>Phương thức khởi tạo trong C# có tên giống với gì?</t>
+  </si>
+  <si>
+    <t>Để comment một dòng trong C# ta sử dụng ký tự nào?</t>
+  </si>
+  <si>
+    <t>Array trong C# bắt đầu từ index nào?</t>
+  </si>
+  <si>
+    <t>Từ khóa nào được sử dụng để khai báo một interface trong C#?</t>
+  </si>
+  <si>
+    <t>Đâu là kiểu dữ liệu giá trị trong C#?</t>
+  </si>
+  <si>
+    <t>Để xử lý ngoại lệ trong C#, ta sử dụng khối lệnh nào?</t>
+  </si>
+  <si>
+    <t>Trong C#, từ khóa "virtual" được sử dụng để làm gì?</t>
+  </si>
+  <si>
+    <t>Phương thức ToString() trong C# có tác dụng gì?</t>
+  </si>
+  <si>
+    <t>Đâu là access modifier trong C#?</t>
+  </si>
+  <si>
+    <t>Để khai báo một mảng trong C#, ta sử dụng ký tự nào?</t>
+  </si>
+  <si>
+    <t>Từ khóa "sealed" trong C# có tác dụng gì?</t>
+  </si>
+  <si>
+    <t>Garbage Collection trong C# là gì?</t>
+  </si>
+  <si>
+    <t>Boxing trong C# là gì?</t>
+  </si>
+  <si>
+    <t>Unboxing trong C# là gì?</t>
+  </si>
+  <si>
+    <t>Delegate trong C# là gì?</t>
+  </si>
+  <si>
+    <t>Event trong C# được sử dụng để làm gì?</t>
+  </si>
+  <si>
+    <t>Generic trong C# là gì?</t>
+  </si>
+  <si>
+    <t>LINQ trong C# là gì?</t>
+  </si>
+  <si>
+    <t>Từ khóa "ref" trong C# được sử dụng để làm gì?</t>
+  </si>
+  <si>
+    <t>Từ khóa "out" trong C# có tác dụng gì?</t>
+  </si>
+  <si>
+    <t>Lambda Expression trong C# là gì?</t>
+  </si>
+  <si>
+    <t>Async/Await trong C# được sử dụng để làm gì?</t>
+  </si>
+  <si>
+    <t>Extension Method trong C# là gì?</t>
+  </si>
+  <si>
+    <t>DapAnA</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>Kết thúc chương trình</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Tạo biến</t>
+  </si>
+  <si>
+    <t>Khai báo biến</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Tên namespace</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>try-catch</t>
+  </si>
+  <si>
+    <t>Chuyển đổi sang chuỗi</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>Ngăn kế thừa</t>
+  </si>
+  <si>
+    <t>Thu gom rác</t>
+  </si>
+  <si>
+    <t>Chuyển value type sang reference type</t>
+  </si>
+  <si>
+    <t>Chuyển reference type sang value type</t>
+  </si>
+  <si>
+    <t>Con trỏ hàm</t>
+  </si>
+  <si>
+    <t>Xử lý sự kiện</t>
+  </si>
+  <si>
+    <t>Kiểu dữ liệu tổng quát</t>
+  </si>
+  <si>
+    <t>Ngôn ngữ truy vấn</t>
+  </si>
+  <si>
+    <t>Truyền tham chiếu</t>
+  </si>
+  <si>
+    <t>Truyền tham chiếu và trả về giá trị</t>
+  </si>
+  <si>
+    <t>Biểu thức hàm ẩn danh</t>
+  </si>
+  <si>
+    <t>Lập trình bất đồng bộ</t>
+  </si>
+  <si>
+    <t>Phương thức mở rộng</t>
+  </si>
+  <si>
+    <t>DapAnB</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>const</t>
+  </si>
+  <si>
+    <t>Điểm bắt đầu chương trình</t>
+  </si>
+  <si>
+    <t>Tổ chức code</t>
+  </si>
+  <si>
+    <t>Import namespace</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>Tên class</t>
+  </si>
+  <si>
+    <t>/* */</t>
+  </si>
+  <si>
+    <t>struct</t>
+  </si>
+  <si>
+    <t>if-else</t>
+  </si>
+  <si>
+    <t>Cho phép ghi đè</t>
+  </si>
+  <si>
+    <t>Tính tổng</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Cho phép kế thừa</t>
+  </si>
+  <si>
+    <t>Xử lý lỗi</t>
+  </si>
+  <si>
+    <t>Tạo mảng</t>
+  </si>
+  <si>
+    <t>Xóa đối tượng</t>
+  </si>
+  <si>
+    <t>Biến cục bộ</t>
+  </si>
+  <si>
+    <t>Tính toán</t>
+  </si>
+  <si>
+    <t>Hằng số</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Vòng lặp</t>
+  </si>
+  <si>
+    <t>Kế thừa</t>
+  </si>
+  <si>
+    <t>DapAnC</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Khởi tạo biến</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Tạo vòng lặp</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Tên biến</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>object</t>
+  </si>
+  <si>
+    <t>switch-case</t>
+  </si>
+  <si>
+    <t>Tạo interface</t>
+  </si>
+  <si>
+    <t>Kiểm tra null</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>Tạo đối tượng</t>
+  </si>
+  <si>
+    <t>Tạo class</t>
+  </si>
+  <si>
+    <t>Thư viện đồ họa</t>
+  </si>
+  <si>
+    <t>Điều kiện</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>DapAnD</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
+    <t>readonly</t>
+  </si>
+  <si>
+    <t>Xử lý ngoại lệ</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>Xử lý file</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>Tên interface</t>
+  </si>
+  <si>
+    <t>##</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>delegate</t>
+  </si>
+  <si>
+    <t>for-while</t>
+  </si>
+  <si>
+    <t>void</t>
+  </si>
+  <si>
+    <t>&lt;&gt;</t>
+  </si>
+  <si>
+    <t>Xử lý chuỗi</t>
+  </si>
+  <si>
+    <t>Xử lý số</t>
+  </si>
+  <si>
+    <t>Cơ sở dữ liệu</t>
+  </si>
+  <si>
+    <t>Mảng</t>
+  </si>
+  <si>
+    <t>Delegate</t>
+  </si>
+  <si>
+    <t>DapAnDung</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -417,13 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4493F3-D16E-4CDF-A8FC-13974AAF6452}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,62 +773,627 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>87</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <v>1</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" t="s">
+        <v>120</v>
+      </c>
+      <c r="F28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>123</v>
+      </c>
+      <c r="F29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>98</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>